<commit_message>
Corrigiendo Documento Product Backlog
</commit_message>
<xml_diff>
--- a/Documentos/PETAPP_BLP_01.xlsx
+++ b/Documentos/PETAPP_BLP_01.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elvis\Documents\Repositorios\Trabajo_Evolucion_Cliente\Documentos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="21015" windowHeight="9690"/>
+    <workbookView xWindow="480" yWindow="330" windowWidth="20730" windowHeight="9690" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -42,9 +37,6 @@
     <t>Pila de Producto (Product Backlog): Instructivo</t>
   </si>
   <si>
-    <t>Elaborado por: pmoinformatica.com</t>
-  </si>
-  <si>
     <t>Estado</t>
   </si>
   <si>
@@ -184,11 +176,14 @@
   <si>
     <t>Backlog del Producto</t>
   </si>
+  <si>
+    <t>Elaborado por: Hans Soto</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -719,7 +714,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -754,7 +749,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -965,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,218 +980,218 @@
   <sheetData>
     <row r="1" spans="2:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="16">
         <v>3</v>
       </c>
       <c r="F4" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>32</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>33</v>
       </c>
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="16">
         <v>3</v>
       </c>
       <c r="F5" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>32</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>33</v>
       </c>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="16">
         <v>2</v>
       </c>
       <c r="F6" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>32</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>33</v>
       </c>
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="16">
         <v>6</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="16">
         <v>2</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="16">
         <v>4</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="16">
         <v>4</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="9"/>
     </row>
     <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="16">
         <v>5</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="18">
         <v>6</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="14"/>
     </row>
@@ -1213,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,7 +1228,7 @@
     </row>
     <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -1249,7 +1244,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="90" x14ac:dyDescent="0.25">
@@ -1257,55 +1252,55 @@
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="225" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizando estados del cuadro excel BackLog del Producto
</commit_message>
<xml_diff>
--- a/Documentos/PETAPP_BLP_01.xlsx
+++ b/Documentos/PETAPP_BLP_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="20730" windowHeight="9690" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="330" windowWidth="20730" windowHeight="9690"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>Columna</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Elaborado por: Hans Soto</t>
+  </si>
+  <si>
+    <t>Realizado</t>
   </si>
 </sst>
 </file>
@@ -960,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,7 +1017,7 @@
         <v>29</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E4" s="16">
         <v>3</v>
@@ -1035,7 +1038,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E5" s="16">
         <v>3</v>
@@ -1077,7 +1080,7 @@
         <v>33</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E7" s="16">
         <v>6</v>
@@ -1098,7 +1101,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E8" s="16">
         <v>2</v>
@@ -1208,7 +1211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>